<commit_message>
bz read and webscarpe working
</commit_message>
<xml_diff>
--- a/newTest2.xlsx
+++ b/newTest2.xlsx
@@ -376,7 +376,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -422,13 +422,13 @@
         <v>bugID</v>
       </c>
       <c r="N1" t="str">
+        <v>IssueLink</v>
+      </c>
+      <c r="O1" t="str">
+        <v>MergeLink</v>
+      </c>
+      <c r="P1" t="str">
         <v>ContainsTheWordFix</v>
-      </c>
-      <c r="O1" t="str">
-        <v>IssueLink</v>
-      </c>
-      <c r="P1" t="str">
-        <v>MergeLink</v>
       </c>
       <c r="Q1" t="str">
         <v>bugType</v>
@@ -494,14 +494,14 @@
       <c r="M2" t="str">
         <v>42717,2815</v>
       </c>
-      <c r="N2">
+      <c r="N2" t="str">
+        <v>https://issues.jenkins-ci.org/browse/JENKINS-42717</v>
+      </c>
+      <c r="O2" t="str">
+        <v>https://github.com/jenkinsci/jenkins/pull/2815</v>
+      </c>
+      <c r="P2">
         <v>2</v>
-      </c>
-      <c r="O2" t="str">
-        <v>https://issues.jenkins-ci.org/browse/JENKINS-42717</v>
-      </c>
-      <c r="P2" t="str">
-        <v>https://github.com/jenkinsci/jenkins/pull/2815</v>
       </c>
       <c r="Q2" t="str">
         <v>bug</v>
@@ -565,14 +565,14 @@
       <c r="M3" t="str">
         <v>42717,2815</v>
       </c>
-      <c r="N3">
+      <c r="N3" t="str">
+        <v>https://issues.jenkins-ci.org/browse/JENKINS-42717</v>
+      </c>
+      <c r="O3" t="str">
+        <v>https://github.com/jenkinsci/jenkins/pull/2815</v>
+      </c>
+      <c r="P3">
         <v>2</v>
-      </c>
-      <c r="O3" t="str">
-        <v>https://issues.jenkins-ci.org/browse/JENKINS-42717</v>
-      </c>
-      <c r="P3" t="str">
-        <v>https://github.com/jenkinsci/jenkins/pull/2815</v>
       </c>
       <c r="Q3" t="str">
         <v>bug</v>
@@ -630,14 +630,14 @@
       <c r="M4" t="str">
         <v>37599,3583</v>
       </c>
-      <c r="N4">
+      <c r="N4" t="str">
+        <v>https://issues.jenkins-ci.org/browse/JENKINS-37599</v>
+      </c>
+      <c r="O4" t="str">
+        <v>https://github.com/jenkinsci/jenkins/pull/3583</v>
+      </c>
+      <c r="P4">
         <v>1</v>
-      </c>
-      <c r="O4" t="str">
-        <v>https://issues.jenkins-ci.org/browse/JENKINS-37599</v>
-      </c>
-      <c r="P4" t="str">
-        <v>https://github.com/jenkinsci/jenkins/pull/3583</v>
       </c>
       <c r="Q4" t="str">
         <v>bug</v>
@@ -693,14 +693,14 @@
       <c r="M5" t="str">
         <v>37599,3583</v>
       </c>
-      <c r="N5">
+      <c r="N5" t="str">
+        <v>https://issues.jenkins-ci.org/browse/JENKINS-37599</v>
+      </c>
+      <c r="O5" t="str">
+        <v>https://github.com/jenkinsci/jenkins/pull/3583</v>
+      </c>
+      <c r="P5">
         <v>1</v>
-      </c>
-      <c r="O5" t="str">
-        <v>https://issues.jenkins-ci.org/browse/JENKINS-37599</v>
-      </c>
-      <c r="P5" t="str">
-        <v>https://github.com/jenkinsci/jenkins/pull/3583</v>
       </c>
       <c r="Q5" t="str">
         <v>bug</v>
@@ -782,14 +782,14 @@
       <c r="M6" t="str">
         <v>3991</v>
       </c>
-      <c r="N6">
+      <c r="N6" t="str">
+        <v/>
+      </c>
+      <c r="O6" t="str">
+        <v>https://github.com/jenkinsci/jenkins/pull/3991</v>
+      </c>
+      <c r="P6">
         <v>2</v>
-      </c>
-      <c r="O6" t="str">
-        <v/>
-      </c>
-      <c r="P6" t="str">
-        <v>https://github.com/jenkinsci/jenkins/pull/3991</v>
       </c>
       <c r="Q6" t="str">
         <v/>
@@ -843,14 +843,14 @@
       <c r="M7" t="str">
         <v>4556</v>
       </c>
-      <c r="N7">
+      <c r="N7" t="str">
+        <v/>
+      </c>
+      <c r="O7" t="str">
+        <v>https://github.com/jenkinsci/jenkins/pull/4556</v>
+      </c>
+      <c r="P7">
         <v>1</v>
-      </c>
-      <c r="O7" t="str">
-        <v/>
-      </c>
-      <c r="P7" t="str">
-        <v>https://github.com/jenkinsci/jenkins/pull/4556</v>
       </c>
       <c r="Q7" t="str">
         <v/>
@@ -860,11 +860,365 @@
       </c>
       <c r="S7" t="str">
         <v/>
+      </c>
+    </row>
+    <row r="8" xml:space="preserve">
+      <c r="A8">
+        <v>25385</v>
+      </c>
+      <c r="B8" t="str">
+        <v>b831acd9854b525d680ca72fd218c848121b9d3f</v>
+      </c>
+      <c r="C8" t="str" xml:space="preserve">
+        <v xml:space="preserve">[JENKINS-42645] Case insensitive search by default for new and anonymous users (#2801)_x000d_
+_x000d_
+* [JENKINS-42645] Case insensitive search by default_x000d__x000d_
+_x000d__x000d_
+* [JENKINS-42960] Search in FixedSet more locale friendly_x000d__x000d_
+_x000d__x000d_
+String.equalsIgnoreCase is safer than toLowerCase when non English_x000d__x000d_
+locales are used._x000d__x000d_
+_x000d__x000d_
+* [JENKINS-42645] Review remarks</v>
+      </c>
+      <c r="D8" t="str">
+        <v>test/src/test/java/jenkins/widgets/HistoryPageFilterCaseSensitiveSearchTest.java</v>
+      </c>
+      <c r="E8">
+        <v>4690</v>
+      </c>
+      <c r="F8">
+        <v>48</v>
+      </c>
+      <c r="G8">
+        <v>35</v>
+      </c>
+      <c r="H8">
+        <v>13</v>
+      </c>
+      <c r="I8" s="1">
+        <v>42832.44458332176</v>
+      </c>
+      <c r="J8" t="str">
+        <v>https://github.com/jenkinsci/jenkins/commit/b831acd9854b525d680ca72fd218c848121b9d3f</v>
+      </c>
+      <c r="K8" t="str">
+        <v>https://github.com/jenkinsci/jenkins/raw/b831acd9854b525d680ca72fd218c848121b9d3f/test/src/test/java/jenkins/widgets/HistoryPageFilterCaseSensitiveSearchTest.java</v>
+      </c>
+      <c r="L8">
+        <v>136</v>
+      </c>
+      <c r="M8" t="str">
+        <v>42645,2801,42960</v>
+      </c>
+      <c r="N8" t="str">
+        <v>https://issues.jenkins-ci.org/browse/JENKINS-42645,https://issues.jenkins-ci.org/browse/JENKINS-42960</v>
+      </c>
+      <c r="O8" t="str">
+        <v>https://github.com/jenkinsci/jenkins/pull/2801</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="str">
+        <v>improvement,bug</v>
+      </c>
+      <c r="R8" t="str">
+        <v>resolved,resolved</v>
+      </c>
+      <c r="S8" t="str">
+        <v>done,fixed</v>
+      </c>
+    </row>
+    <row r="9" xml:space="preserve">
+      <c r="A9">
+        <v>6297</v>
+      </c>
+      <c r="B9" t="str">
+        <v>312fcd1b9ebb5f4ce396c2b7cc93659edd6301c1</v>
+      </c>
+      <c r="C9" t="str" xml:space="preserve">
+        <v xml:space="preserve">[JENKINS-54854] Added a warning when cron trigger spent more than a threshold (30s) in its execution (#3802)_x000d_
+_x000d_
+* [JENKINS-54854] Added a warning when cron trigger spent more than a threshold (30s) in its execution_x000d__x000d_
+_x000d__x000d_
+* Added a test_x000d__x000d_
+_x000d__x000d_
+* Fix based on feedback_x000d__x000d_
+_x000d__x000d_
+* Added Admin monitor_x000d__x000d_
+_x000d__x000d_
+* Cleanup_x000d__x000d_
+_x000d__x000d_
+* Polishing_x000d__x000d_
+_x000d__x000d_
+* Fix according the feedback provided by Oliver_x000d__x000d_
+_x000d__x000d_
+* Added missing renamed admin monitor class_x000d__x000d_
+_x000d__x000d_
+* Better Web layout_x000d__x000d_
+_x000d__x000d_
+* Limit stacked messages to 10 by default_x000d__x000d_
+_x000d__x000d_
+* Improved replacement_x000d__x000d_
+_x000d__x000d_
+* Make SlowTriggerAdminMonitor#errors thread-safe_x000d__x000d_
+_x000d__x000d_
+* Fixed as requested_x000d__x000d_
+_x000d__x000d_
+* Admin monitor title changed</v>
+      </c>
+      <c r="D9" t="str">
+        <v>test/src/test/java/jenkins/triggers/TriggerTest.java</v>
+      </c>
+      <c r="E9">
+        <v>1160</v>
+      </c>
+      <c r="F9">
+        <v>118</v>
+      </c>
+      <c r="G9">
+        <v>118</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>43673.3347337963</v>
+      </c>
+      <c r="J9" t="str">
+        <v>https://github.com/jenkinsci/jenkins/commit/312fcd1b9ebb5f4ce396c2b7cc93659edd6301c1</v>
+      </c>
+      <c r="K9" t="str">
+        <v>https://github.com/jenkinsci/jenkins/raw/312fcd1b9ebb5f4ce396c2b7cc93659edd6301c1/test/src/test/java/jenkins/triggers/TriggerTest.java</v>
+      </c>
+      <c r="L9">
+        <v>117</v>
+      </c>
+      <c r="M9" t="str">
+        <v>54854,3802</v>
+      </c>
+      <c r="N9" t="str">
+        <v>https://issues.jenkins-ci.org/browse/JENKINS-54854</v>
+      </c>
+      <c r="O9" t="str">
+        <v>https://github.com/jenkinsci/jenkins/pull/3802</v>
+      </c>
+      <c r="P9">
+        <v>3</v>
+      </c>
+      <c r="Q9" t="str">
+        <v>improvement</v>
+      </c>
+      <c r="R9" t="str">
+        <v>resolved</v>
+      </c>
+      <c r="S9" t="str">
+        <v>fixed</v>
+      </c>
+    </row>
+    <row r="10" xml:space="preserve">
+      <c r="A10">
+        <v>20160</v>
+      </c>
+      <c r="B10" t="str">
+        <v>a79fdaa4b34b8f7fddb39bed3eabf4763940d11b</v>
+      </c>
+      <c r="C10" t="str" xml:space="preserve">
+        <v xml:space="preserve">Revert "[JENKINS-46911] createProjectFromXML not recognizing unsafe character…" (#3218)_x000d_
+_x000d_
+* Revert "[JENKINS-48447] Fixed HTTP 404 error when clicking on newView sidebar link from an other view. (#3178)"_x000d__x000d_
+_x000d__x000d_
+This reverts commit 6df06fc19a4b7ed015ab5213e2dc8d25beb2f607._x000d__x000d_
+_x000d__x000d_
+* Revert "[JENKINS-46911] createProjectFromXML not recognizing unsafe character… (#3057)"_x000d__x000d_
+_x000d__x000d_
+This reverts commit ac2a1aaf895020bc80fd951ced748820975df6aa.</v>
+      </c>
+      <c r="D10" t="str">
+        <v>test/src/test/java/jenkins/triggers/ReverseBuildTriggerTest.java</v>
+      </c>
+      <c r="E10">
+        <v>3552</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1">
+        <v>43107.76871527778</v>
+      </c>
+      <c r="J10" t="str">
+        <v>https://github.com/jenkinsci/jenkins/commit/a79fdaa4b34b8f7fddb39bed3eabf4763940d11b</v>
+      </c>
+      <c r="K10" t="str">
+        <v>https://github.com/jenkinsci/jenkins/raw/a79fdaa4b34b8f7fddb39bed3eabf4763940d11b/test/src/test/java/jenkins/triggers/ReverseBuildTriggerTest.java</v>
+      </c>
+      <c r="L10">
+        <v>243</v>
+      </c>
+      <c r="M10" t="str">
+        <v>46911,3218,48447,3178,3057</v>
+      </c>
+      <c r="N10" t="str">
+        <v>https://issues.jenkins-ci.org/browse/JENKINS-46911,https://issues.jenkins-ci.org/browse/JENKINS-48447</v>
+      </c>
+      <c r="O10" t="str">
+        <v>https://github.com/jenkinsci/jenkins/pull/3218,https://github.com/jenkinsci/jenkins/pull/3178,https://github.com/jenkinsci/jenkins/pull/3057</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10" t="str">
+        <v>bug,bug</v>
+      </c>
+      <c r="R10" t="str">
+        <v>open,resolved</v>
+      </c>
+      <c r="S10" t="str">
+        <v>unresolved,fixed</v>
+      </c>
+    </row>
+    <row r="11" xml:space="preserve">
+      <c r="A11">
+        <v>20358</v>
+      </c>
+      <c r="B11" t="str">
+        <v>ac2a1aaf895020bc80fd951ced748820975df6aa</v>
+      </c>
+      <c r="C11" t="str" xml:space="preserve">
+        <v xml:space="preserve">[JENKINS-46911] createProjectFromXML not recognizing unsafe character… (#3057)_x000d_
+_x000d_
+* [JENKINS-46911] createProjectFromXML not recognizing unsafe character '/'_x000d__x000d_
+_x000d__x000d_
+* Better place for testCreateProjectCheckGoodName()_x000d__x000d_
+_x000d__x000d_
+* Fix failed test_x000d__x000d_
+_x000d__x000d_
+* Make changes suggested on PR review._x000d__x000d_
+_x000d__x000d_
+* Remove Failure exception, instead throw IOException. Add javadoc_x000d__x000d_
+_x000d__x000d_
+* [JENKINS-46911] - Add TODO according to the comment from @jtnord.</v>
+      </c>
+      <c r="D11" t="str">
+        <v>test/src/test/java/jenkins/triggers/ReverseBuildTriggerTest.java</v>
+      </c>
+      <c r="E11">
+        <v>3548</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1">
+        <v>43107.61053240741</v>
+      </c>
+      <c r="J11" t="str">
+        <v>https://github.com/jenkinsci/jenkins/commit/ac2a1aaf895020bc80fd951ced748820975df6aa</v>
+      </c>
+      <c r="K11" t="str">
+        <v>https://github.com/jenkinsci/jenkins/raw/ac2a1aaf895020bc80fd951ced748820975df6aa/test/src/test/java/jenkins/triggers/ReverseBuildTriggerTest.java</v>
+      </c>
+      <c r="L11">
+        <v>243</v>
+      </c>
+      <c r="M11" t="str">
+        <v>46911,3057</v>
+      </c>
+      <c r="N11" t="str">
+        <v>https://issues.jenkins-ci.org/browse/JENKINS-46911</v>
+      </c>
+      <c r="O11" t="str">
+        <v>https://github.com/jenkinsci/jenkins/pull/3057</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11" t="str">
+        <v>bug</v>
+      </c>
+      <c r="R11" t="str">
+        <v>open</v>
+      </c>
+      <c r="S11" t="str">
+        <v>unresolved</v>
+      </c>
+    </row>
+    <row r="12" xml:space="preserve">
+      <c r="A12">
+        <v>20927</v>
+      </c>
+      <c r="B12" t="str">
+        <v>2ae37219fe635d1a93d1bb9a6ad5d79cc4072489</v>
+      </c>
+      <c r="C12" t="str" xml:space="preserve">
+        <v xml:space="preserve">Merge pull request #3000 from liketic/JENKINS-46161_x000d_
+_x000d_
+[Fix JENKINS-46161] Make ReverseBuildTrigger#getUpstreamProjects null…</v>
+      </c>
+      <c r="D12" t="str">
+        <v>test/src/test/java/jenkins/triggers/ReverseBuildTriggerTest.java</v>
+      </c>
+      <c r="E12">
+        <v>4146</v>
+      </c>
+      <c r="F12">
+        <v>16</v>
+      </c>
+      <c r="G12">
+        <v>16</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>42993.77978009259</v>
+      </c>
+      <c r="J12" t="str">
+        <v>https://github.com/jenkinsci/jenkins/commit/2ae37219fe635d1a93d1bb9a6ad5d79cc4072489</v>
+      </c>
+      <c r="K12" t="str">
+        <v>https://github.com/jenkinsci/jenkins/raw/2ae37219fe635d1a93d1bb9a6ad5d79cc4072489/test/src/test/java/jenkins/triggers/ReverseBuildTriggerTest.java</v>
+      </c>
+      <c r="L12">
+        <v>243</v>
+      </c>
+      <c r="M12" t="str">
+        <v>3000,46161</v>
+      </c>
+      <c r="N12" t="str">
+        <v>https://issues.jenkins-ci.org/browse/JENKINS-46161</v>
+      </c>
+      <c r="O12" t="str">
+        <v>https://github.com/jenkinsci/jenkins/pull/3000</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12" t="str">
+        <v>improvement</v>
+      </c>
+      <c r="R12" t="str">
+        <v>closed</v>
+      </c>
+      <c r="S12" t="str">
+        <v>fixed</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:S7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:S12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>